<commit_message>
as-is e matrizes para to-be da vendas geral unificada
</commit_message>
<xml_diff>
--- a/as-is-documentation/venda-geral.xlsx
+++ b/as-is-documentation/venda-geral.xlsx
@@ -1198,10 +1198,10 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="N23 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.09"/>
@@ -1399,10 +1399,10 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="1" sqref="N23 A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="62.57"/>
@@ -1763,10 +1763,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="N23" activeCellId="0" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.09"/>
@@ -2063,7 +2063,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="38" t="s">
         <v>111</v>
       </c>
       <c r="K9" s="30"/>
@@ -2107,7 +2107,7 @@
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="38" t="s">
         <v>111</v>
       </c>
       <c r="G11" s="30"/>
@@ -2132,7 +2132,7 @@
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="38" t="s">
         <v>112</v>
       </c>
       <c r="G12" s="30"/>
@@ -2148,7 +2148,7 @@
       <c r="P12" s="30"/>
       <c r="Q12" s="30"/>
       <c r="R12" s="30"/>
-      <c r="S12" s="32" t="s">
+      <c r="S12" s="38" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2194,7 +2194,7 @@
       <c r="M14" s="35"/>
       <c r="O14" s="35"/>
       <c r="P14" s="35"/>
-      <c r="Q14" s="31" t="s">
+      <c r="Q14" s="38" t="s">
         <v>111</v>
       </c>
       <c r="R14" s="35"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="31" t="s">
         <v>111</v>
       </c>
       <c r="I20" s="30"/>
@@ -2630,7 +2630,7 @@
       <c r="B31" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="17" t="s">
         <v>112</v>
       </c>
       <c r="D31" s="30"/>
@@ -2644,7 +2644,7 @@
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
       <c r="L31" s="30"/>
-      <c r="M31" s="34" t="s">
+      <c r="M31" s="17" t="s">
         <v>112</v>
       </c>
       <c r="N31" s="30"/>

</xml_diff>